<commit_message>
spare parts table and single logitems in man_hrs
</commit_message>
<xml_diff>
--- a/FinalResults/flight_maintenance_description_result.xlsx
+++ b/FinalResults/flight_maintenance_description_result.xlsx
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['HMV23/000059/0923/3', 'HMV23/000055/0923/17']</t>
+          <t>['HMV23/000055/0923/17', 'HMV23/000059/0923/3']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['DURING ARRIVAL INSPECTION FOUND STATIC DISCHARGERS DAMAGED AT LOCATION : \n1) LH HORZ STAB TYPE A DISCHARGER QTY# 2 &amp; TYPE B DISCHARGER QTY#3 \n2) RH HORZ STAB TYPE A DISCHARGER QTY#1 \n3)VERTICAL STABILISER TYPE A DISCHARGER QTY 01 &amp; TYPE B DISCHARGER QTY 02.', 'DURING ARRIVAL INSPECTION FOUND STATIC DISCHARGERS DAMAGED AT LOCATION LH WING TIP TRAILING EDGE TYPE B DISCHARGER QTY#1, RH HORZ STAB TYPE A DISCHARGER QTY#1 TYPE B DISCHARGER QTY#1, LH HORZ STAB TYPE A DISCHARGER QTY#1 TYPE B DISCHARGER QTY#3, VERT STAB TYPE A DISCHARGER QTY#1, RUDDER TYPE B DISCHARGER QTY#1.']</t>
+          <t>['DURING ARRIVAL INSPECTION FOUND STATIC DISCHARGERS DAMAGED AT LOCATION LH WING TIP TRAILING EDGE TYPE B DISCHARGER QTY#1, RH HORZ STAB TYPE A DISCHARGER QTY#1 TYPE B DISCHARGER QTY#1, LH HORZ STAB TYPE A DISCHARGER QTY#1 TYPE B DISCHARGER QTY#3, VERT STAB TYPE A DISCHARGER QTY#1, RUDDER TYPE B DISCHARGER QTY#1.', 'DURING ARRIVAL INSPECTION FOUND STATIC DISCHARGERS DAMAGED AT LOCATION : \n1) LH HORZ STAB TYPE A DISCHARGER QTY# 2 &amp; TYPE B DISCHARGER QTY#3 \n2) RH HORZ STAB TYPE A DISCHARGER QTY#1 \n3)VERTICAL STABILISER TYPE A DISCHARGER QTY 01 &amp; TYPE B DISCHARGER QTY 02.']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[5.0, 7.0]</t>
+          <t>[7.0, 5.0]</t>
         </is>
       </c>
     </row>
@@ -485,12 +485,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['HMV23/000055/0923/21', 'HMV23/000059/0923/4']</t>
+          <t>['HMV23/000059/0923/4', 'HMV23/000055/0923/21']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['DURING ARRIVAL CHECK FOUND SERVICE LIGHT LAMP INOP AT FOLLOWING LOCATION\n1. 80VU RH AVIONICS COMPARTMENT FIN: 9LS QTY#1, 90VU FWD AVIONICS COMPARMENT FIN: 6LS QTY#1.\n2. THS COMPARMENT FIN: 5LJ QTY#1.', 'DURING ARRIVAL CHECK FOUND SERVICE LIGHT LAMP INOP AT FOLLOWING LOCATION \n1.103VU BATTERY COMPARMENT LAMP FIN: 8LS QTY#1,.\n2. REFUEL/DEFUEL CONTROL PANEL FLOODLIGHT LAMP FIN: 32QU.']</t>
+          <t>['DURING ARRIVAL CHECK FOUND SERVICE LIGHT LAMP INOP AT FOLLOWING LOCATION \n1.103VU BATTERY COMPARMENT LAMP FIN: 8LS QTY#1,.\n2. REFUEL/DEFUEL CONTROL PANEL FLOODLIGHT LAMP FIN: 32QU.', 'DURING ARRIVAL CHECK FOUND SERVICE LIGHT LAMP INOP AT FOLLOWING LOCATION\n1. 80VU RH AVIONICS COMPARTMENT FIN: 9LS QTY#1, 90VU FWD AVIONICS COMPARMENT FIN: 6LS QTY#1.\n2. THS COMPARMENT FIN: 5LJ QTY#1.']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['HMV23/000059/0923/5', 'HMV23/000055/0923/6', 'HMV23/000055/0923/2', 'HMV23/000043/0823/12']</t>
+          <t>['HMV23/000059/0923/5', 'HMV23/000055/0923/2', 'HMV23/000043/0823/12', 'HMV23/000055/0923/6']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['DURING ARRIVAL INSPECTION , OBSERVED FOLLOWINS DICREPANCIES.\n\n1) RH SIDE WING NO#1 SLAT, NO.3 TRACK SQURE SEAL UPPER BULB SEAL DEGRADED.\n2) RH SIIDE WING SLAT NO#5 OUT BOARD WEATHER SEAL ERODED. SAME TO BE REPLACED.', 'DURING INSPECTION, OBSERVED RH SIDE WING SLAT NO#5 WEATHER SEAL ERODED.SAME TO BE REPLACED.', 'DURING INSPECTION OBSERVED LH WING SLAT#5 WEATHER SEAL ERODED.SAME TO BE REPLACED.', 'WHILE ARRIVAL INSPECTION OBSERVED RH WING SLAT#5 OUTBOARD WEATHER SEAL ERODED.SAME TO BE REPLACED.']</t>
+          <t>['DURING ARRIVAL INSPECTION , OBSERVED FOLLOWINS DICREPANCIES.\n\n1) RH SIDE WING NO#1 SLAT, NO.3 TRACK SQURE SEAL UPPER BULB SEAL DEGRADED.\n2) RH SIIDE WING SLAT NO#5 OUT BOARD WEATHER SEAL ERODED. SAME TO BE REPLACED.', 'DURING INSPECTION OBSERVED LH WING SLAT#5 WEATHER SEAL ERODED.SAME TO BE REPLACED.', 'WHILE ARRIVAL INSPECTION OBSERVED RH WING SLAT#5 OUTBOARD WEATHER SEAL ERODED.SAME TO BE REPLACED.', 'DURING INSPECTION, OBSERVED RH SIDE WING SLAT NO#5 WEATHER SEAL ERODED.SAME TO BE REPLACED.']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[0.0, 3.0, 2.0, 2.0]</t>
+          <t>[0.0, 2.0, 2.0, 3.0]</t>
         </is>
       </c>
     </row>
@@ -529,12 +529,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['HMV23/000055/0923/11', 'HMV23/000059/0923/6']</t>
+          <t>['HMV23/000059/0923/6', 'HMV23/000055/0923/11']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['DURING INSPECTION FOUND FOLLOWING FORWARD CARGO FLOOR PANEL DAMAGED , TO BE FABRICATED/REPLACED \n\n131 AF P/N D5367520400000\n\n131EF P/N D5367521000000\n\n131FF P/N D5367400800000\n\n131BF P/N D5367401200000\n\n131CF P/N D5367401100000\n\n131GF P/N D5367400700000', 'DURING INSPECTION FOUND FOLLOWING FORWARD CARGO FLOOR PANEL DAMAGED , TO BE FABRICATED/REPLACED \n\n\n\n131EF P/N D5367521000000 \n\n131FF P/N D5367400800000 \n\n131BF P/N D5367401200000 \n\n131JF P/N D5367400600000']</t>
+          <t>['DURING INSPECTION FOUND FOLLOWING FORWARD CARGO FLOOR PANEL DAMAGED , TO BE FABRICATED/REPLACED \n\n\n\n131EF P/N D5367521000000 \n\n131FF P/N D5367400800000 \n\n131BF P/N D5367401200000 \n\n131JF P/N D5367400600000', 'DURING INSPECTION FOUND FOLLOWING FORWARD CARGO FLOOR PANEL DAMAGED , TO BE FABRICATED/REPLACED \n\n131 AF P/N D5367520400000\n\n131EF P/N D5367521000000\n\n131FF P/N D5367400800000\n\n131BF P/N D5367401200000\n\n131CF P/N D5367401100000\n\n131GF P/N D5367400700000']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -573,17 +573,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['HMV23/000059/0923/9', 'HMV23/000055/0923/13', 'HMV23/000059/0923/8', 'HMV23/000055/0923/14']</t>
+          <t>['HMV23/000059/0923/8', 'HMV23/000055/0923/14', 'HMV23/000055/0923/13', 'HMV23/000059/0923/9']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['DURING ARRIVAL INSPECTION OF AFT CARGO , FOUND \n1) CARGO SECTION HOSE MISSING/ DAMAGED \n2) FOUND HARDWARE DAMAGED/MISSING', 'DURING ARRIVAL INSPECTION OF FORWARD CARGO , FOUND \n1) CARGO SECTION HOSE MISSING/ DAMAGED \n2) FOUND HARDWARE DAMAGED/MISSING', 'DURING ARRIVAL INSPECTION OF FORWARD CARGO , FOUND HARDWARE DAMAGED/MISSING', 'DURING ARRIVAL INSPECTION OF AFT CARGO , FOUND \n1) CARGO SECTION HOSE MISSING/ DAMAGED \n2) FOUND HARDWARE DAMAGED/MISSING']</t>
+          <t>['DURING ARRIVAL INSPECTION OF FORWARD CARGO , FOUND HARDWARE DAMAGED/MISSING', 'DURING ARRIVAL INSPECTION OF AFT CARGO , FOUND \n1) CARGO SECTION HOSE MISSING/ DAMAGED \n2) FOUND HARDWARE DAMAGED/MISSING', 'DURING ARRIVAL INSPECTION OF FORWARD CARGO , FOUND \n1) CARGO SECTION HOSE MISSING/ DAMAGED \n2) FOUND HARDWARE DAMAGED/MISSING', 'DURING ARRIVAL INSPECTION OF AFT CARGO , FOUND \n1) CARGO SECTION HOSE MISSING/ DAMAGED \n2) FOUND HARDWARE DAMAGED/MISSING']</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[7.0, 5.0, 5.0, 5.0]</t>
+          <t>[5.0, 5.0, 5.0, 7.0]</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['HMV23/000059/0923/15', 'HMV23/000055/0923/10']</t>
+          <t>['HMV23/000055/0923/10', 'HMV23/000059/0923/15']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['DURING ARRIVAL CHECK FOUND EPSU BATTERIES QTY#2 FIN:10WL AND FIN: 11WL INOP.', 'DURING WEEKLY INSPECTION OBSERVED FIN: 11WL EPSU BATTERY INOP.']</t>
+          <t>['DURING WEEKLY INSPECTION OBSERVED FIN: 11WL EPSU BATTERY INOP.', 'DURING ARRIVAL CHECK FOUND EPSU BATTERIES QTY#2 FIN:10WL AND FIN: 11WL INOP.']</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[6.0, 5.0]</t>
+          <t>[5.0, 6.0]</t>
         </is>
       </c>
     </row>
@@ -683,17 +683,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['HMV23/000059/0923/16', 'HMV23/000055/0923/23']</t>
+          <t>['HMV23/000055/0923/23', 'HMV23/000059/0923/16']</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['DURING WEAR LIMIT BONDING LEADS INSPECTION CHECK FOUND BONDING LEADS DAMAGED AT LOCATION TOILET SERVICE PANEL QTY#1, WATER SERVICE PANEL QTY#2, RH MLG DOOR QTY#1, LH MLG DOOR QTY#1, LH ELEVATOR QTY#3, RH ELEVATOR QTY#1, RH WING BETWEEN SPOILER 3 AND 4 QTY#2, LH WING FLAP TRACK FAIRING NO.3 QTY#1, RH WING FLAP TRACK FAIRING NO.1 QTY#2.', 'DURING WEAR LIMIT BONDING LEADS INSPECTION CHECK FOUND BONDING LEADS DAMAGED AT LOCATION TOILET SERVICE PANEL QTY#2, WATER SERVICE PANEL QTY#2, RH MLG DOOR QTY#1, LH MLG DOOR QTY#2, 108VU QTY#1, FWD CARGO DOOR QTY#1, AFT CARGO DOOR QTY#1, FWD LH PASSENGER DOOR QTY#1, RH WING FLAP TRACK FAIRING NO.2 QTY#1, RH WING FLAP TRACK FAIRING NO.3 QTY#1, LH WING FLAP TRACK FAIRING NO.1 QTY#2, LH WING FLAP TRACK FAIRING NO.3 QTY#2, LH ELEVATOR PANEL 334BB QTY#1, LH ELEVATOR PANEL 334HB QTY#1, RH ELEVATOR PANEL 344DB QTY#1, RH ELEVATOR PANEL 344BB QTY#1.']</t>
+          <t>['DURING WEAR LIMIT BONDING LEADS INSPECTION CHECK FOUND BONDING LEADS DAMAGED AT LOCATION TOILET SERVICE PANEL QTY#2, WATER SERVICE PANEL QTY#2, RH MLG DOOR QTY#1, LH MLG DOOR QTY#2, 108VU QTY#1, FWD CARGO DOOR QTY#1, AFT CARGO DOOR QTY#1, FWD LH PASSENGER DOOR QTY#1, RH WING FLAP TRACK FAIRING NO.2 QTY#1, RH WING FLAP TRACK FAIRING NO.3 QTY#1, LH WING FLAP TRACK FAIRING NO.1 QTY#2, LH WING FLAP TRACK FAIRING NO.3 QTY#2, LH ELEVATOR PANEL 334BB QTY#1, LH ELEVATOR PANEL 334HB QTY#1, RH ELEVATOR PANEL 344DB QTY#1, RH ELEVATOR PANEL 344BB QTY#1.', 'DURING WEAR LIMIT BONDING LEADS INSPECTION CHECK FOUND BONDING LEADS DAMAGED AT LOCATION TOILET SERVICE PANEL QTY#1, WATER SERVICE PANEL QTY#2, RH MLG DOOR QTY#1, LH MLG DOOR QTY#1, LH ELEVATOR QTY#3, RH ELEVATOR QTY#1, RH WING BETWEEN SPOILER 3 AND 4 QTY#2, LH WING FLAP TRACK FAIRING NO.3 QTY#1, RH WING FLAP TRACK FAIRING NO.1 QTY#2.']</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[18.0, 24.0]</t>
+          <t>[24.0, 18.0]</t>
         </is>
       </c>
     </row>
@@ -727,17 +727,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['HMV23/000055/0923/8', 'HMV23/000055/0923/7', 'HMV23/000055/0923/1', 'HMV23/000055/0923/9']</t>
+          <t>['HMV23/000055/0923/1', 'HMV23/000055/0923/7', 'HMV23/000055/0923/9', 'HMV23/000055/0923/8']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['DURING ARRIVAL INSPECTION, OBSERVED SMALL DENTS ON SLAT NO #1 TOP SKIN AT RH SIDE WING. LOCATION OF DENT 3.5 INCH FROM T/E AND 37 INCH FROM INBD EDGE OF SLAT.\nSLAT NO#1 P/N- D5746091000300\n S/N- SA7205917', 'DURING ARRIVAL INSPECTION , OBSERVED DENT ON SLAT NO #2 LIP AREA AT RH SIDE WING. DENT LOCATION, 3 INCH FROM T/E AND 67.5 INCH FROM OUTBD EDGE .ASSESSMENT TO BE CARRY OUT.\nSLAT NO #2 P/N- D5746092000500\n S/N- SA7205698', 'DURING ARRIVAL INSPECTION , OBSERVED DENT ON SLAT NO #2 LIP AREA AT RH SIDE WING. ASSESSMENT TO BE CARRY OUT.\n\nSLAT NO #2 P/N- D5746092000500\n SA7205698', 'DURING ARRIVAL INSPECTION, OBSERVED SMALL DENTS ON SLAT NO #1 TOP SKIN AT RH SIDE WING. LOCATION OF DENT 3.5 INCH FROM T/E AND 37 INCH FROM INBD EDGE OF SLAT.\nSLAT NO#1 P/N- D5746091000300\n S/N- SA7205917']</t>
+          <t>['DURING ARRIVAL INSPECTION , OBSERVED DENT ON SLAT NO #2 LIP AREA AT RH SIDE WING. ASSESSMENT TO BE CARRY OUT.\n\nSLAT NO #2 P/N- D5746092000500\n SA7205698', 'DURING ARRIVAL INSPECTION , OBSERVED DENT ON SLAT NO #2 LIP AREA AT RH SIDE WING. DENT LOCATION, 3 INCH FROM T/E AND 67.5 INCH FROM OUTBD EDGE .ASSESSMENT TO BE CARRY OUT.\nSLAT NO #2 P/N- D5746092000500\n S/N- SA7205698', 'DURING ARRIVAL INSPECTION, OBSERVED SMALL DENTS ON SLAT NO #1 TOP SKIN AT RH SIDE WING. LOCATION OF DENT 3.5 INCH FROM T/E AND 37 INCH FROM INBD EDGE OF SLAT.\nSLAT NO#1 P/N- D5746091000300\n S/N- SA7205917', 'DURING ARRIVAL INSPECTION, OBSERVED SMALL DENTS ON SLAT NO #1 TOP SKIN AT RH SIDE WING. LOCATION OF DENT 3.5 INCH FROM T/E AND 37 INCH FROM INBD EDGE OF SLAT.\nSLAT NO#1 P/N- D5746091000300\n S/N- SA7205917']</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[3.0, 7.0, 2.0, 7.0]</t>
+          <t>[2.0, 7.0, 7.0, 3.0]</t>
         </is>
       </c>
     </row>
@@ -749,17 +749,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['HMV23/000055/0923/5', 'HMV23/000055/0923/3', 'HMV23/000055/0923/4']</t>
+          <t>['HMV23/000055/0923/4', 'HMV23/000055/0923/3', 'HMV23/000055/0923/5']</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['DURING ARRIVAL INSPECTION FOUND FOLLOWING FAILURE MSG IN PFR:\n1. 38-31-41 TOILET ASSY LAV F\nFURTHER RECTIFICATION TO BE CARRIED OUT.', 'DURING ARRIVAL INSPECTION FOUND FOLLOWING WARNING MSG IN PFR:\n1. AUTO FLT AP OFF\nFURTHER RECTIFICATION TO BE CARRIED OUT.', 'DURING ARRIVAL INSPECTION FOUND FOLLOWING FAILURE MSG IN PFR:\n1. 34-53-31 ADF1(2RP1)\nFURTHER RECTIFICATION TO BE CARRIED OUT.']</t>
+          <t>['DURING ARRIVAL INSPECTION FOUND FOLLOWING FAILURE MSG IN PFR:\n1. 34-53-31 ADF1(2RP1)\nFURTHER RECTIFICATION TO BE CARRIED OUT.', 'DURING ARRIVAL INSPECTION FOUND FOLLOWING WARNING MSG IN PFR:\n1. AUTO FLT AP OFF\nFURTHER RECTIFICATION TO BE CARRIED OUT.', 'DURING ARRIVAL INSPECTION FOUND FOLLOWING FAILURE MSG IN PFR:\n1. 38-31-41 TOILET ASSY LAV F\nFURTHER RECTIFICATION TO BE CARRIED OUT.']</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[4.0, 2.0, 2.5]</t>
+          <t>[2.5, 2.0, 4.0]</t>
         </is>
       </c>
     </row>

</xml_diff>